<commit_message>
EPBDS: fixed the following bug mapping rule is not processed properly if destination field path is deep mapping path and contains index operator in the middle (it is bug is applicable for Acord's types)
</commit_message>
<xml_diff>
--- a/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/hints/FieldHintsSupportTest.xlsx
+++ b/MAPPING/trunk/org.openl.rules.mapping.dev/src/test/resources/org/openl/rules/mapping/hints/FieldHintsSupportTest.xlsx
@@ -41,9 +41,6 @@
     <t>org.openl.rules.mapping</t>
   </si>
   <si>
-    <t>org.openuri.easypo</t>
-  </si>
-  <si>
     <t>Class A</t>
   </si>
   <si>
@@ -107,43 +104,46 @@
     <t>org.openl.rules.mapping.to</t>
   </si>
   <si>
+    <t>ChildA,A</t>
+  </si>
+  <si>
+    <t>fieldAType</t>
+  </si>
+  <si>
+    <t>fieldBType</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>ChildA</t>
+  </si>
+  <si>
+    <t>oneWay</t>
+  </si>
+  <si>
+    <t>ChildA,ChildA</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>ChildA, A</t>
+  </si>
+  <si>
+    <t>//Data Mapping mappings2</t>
+  </si>
+  <si>
+    <t>array[6]</t>
+  </si>
+  <si>
+    <t>array[7]</t>
+  </si>
+  <si>
+    <t>org.openl.rules.mapping.to.containers</t>
+  </si>
+  <si>
     <t>org.openl.rules.mapping.to.inheritance</t>
-  </si>
-  <si>
-    <t>ChildA,A</t>
-  </si>
-  <si>
-    <t>fieldAType</t>
-  </si>
-  <si>
-    <t>fieldBType</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>ChildA</t>
-  </si>
-  <si>
-    <t>oneWay</t>
-  </si>
-  <si>
-    <t>ChildA,ChildA</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>ChildA, A</t>
-  </si>
-  <si>
-    <t>//Data Mapping mappings2</t>
-  </si>
-  <si>
-    <t>array[6]</t>
-  </si>
-  <si>
-    <t>array[7]</t>
   </si>
 </sst>
 </file>
@@ -293,43 +293,43 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="C8:K26"/>
+  <dimension ref="C4:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -643,273 +643,273 @@
     <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="4" spans="3:11">
+      <c r="C4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="3:11">
+      <c r="C5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11">
+      <c r="C6" s="8"/>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11">
+      <c r="C7" s="8"/>
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="8" spans="3:11">
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="3:11">
-      <c r="C9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="3:11">
-      <c r="C10" s="4"/>
-      <c r="D10" s="1" t="s">
+      <c r="C8" s="8"/>
+      <c r="D8" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11">
+      <c r="C12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="3:11">
+      <c r="C13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11">
+      <c r="C14" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="3:11">
-      <c r="C11" s="4"/>
-      <c r="D11" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="3:11">
-      <c r="C12" s="4"/>
-      <c r="D12" s="1" t="s">
+      <c r="D14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="13"/>
+      <c r="I14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>30</v>
       </c>
+      <c r="K14" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11">
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
     </row>
     <row r="16" spans="3:11">
-      <c r="C16" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="14"/>
     </row>
     <row r="17" spans="3:11">
-      <c r="C17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G17" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="12"/>
-      <c r="I17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J17" s="2" t="s">
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="14"/>
+    </row>
+    <row r="18" spans="3:11">
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" t="s">
+        <v>26</v>
+      </c>
+      <c r="G18" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11">
+      <c r="C19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="3:11">
-      <c r="C18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="13" t="s">
+      <c r="K19" s="14"/>
+    </row>
+    <row r="20" spans="3:11">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="H18" s="14"/>
-      <c r="I18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K18" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="3:11">
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="15"/>
-      <c r="H19" s="15"/>
-    </row>
-    <row r="20" spans="3:11">
-      <c r="C20" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="9"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="14"/>
     </row>
     <row r="21" spans="3:11">
       <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
         <v>17</v>
-      </c>
-      <c r="D21" t="s">
-        <v>18</v>
       </c>
       <c r="E21" t="s">
         <v>22</v>
       </c>
       <c r="F21" t="s">
-        <v>26</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21" s="9"/>
+        <v>39</v>
+      </c>
+      <c r="G21" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="14"/>
     </row>
     <row r="22" spans="3:11">
       <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
         <v>17</v>
-      </c>
-      <c r="D22" t="s">
-        <v>18</v>
       </c>
       <c r="E22" t="s">
         <v>23</v>
       </c>
       <c r="F22" t="s">
-        <v>27</v>
-      </c>
-      <c r="G22" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="3:11">
-      <c r="C23" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="3:11">
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="9"/>
-    </row>
-    <row r="25" spans="3:11">
-      <c r="C25" t="s">
-        <v>17</v>
-      </c>
-      <c r="D25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" t="s">
-        <v>23</v>
-      </c>
-      <c r="F25" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H25" s="9"/>
-    </row>
-    <row r="26" spans="3:11">
-      <c r="C26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" t="s">
-        <v>42</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H26" s="9"/>
-      <c r="K26" t="s">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H22" s="14"/>
+      <c r="K22" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="K23:K24"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G15:H15"/>
     <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G20:H20"/>
     <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C16:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -936,17 +936,17 @@
   </cols>
   <sheetData>
     <row r="7" spans="3:12">
-      <c r="C7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="C7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="3:12">
       <c r="C8" s="2" t="s">
@@ -961,103 +961,101 @@
       <c r="F8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="G8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="12"/>
-      <c r="I8" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="J8" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="3:12">
       <c r="C9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="14"/>
+      <c r="G9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="13"/>
       <c r="I9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="3:12">
-      <c r="C10" s="9" t="s">
-        <v>18</v>
+      <c r="C10" s="14" t="s">
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="14"/>
       <c r="I10" s="15"/>
       <c r="J10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K10" s="15"/>
-      <c r="L10" s="9" t="b">
+      <c r="L10" s="14" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="3:12">
-      <c r="C11" s="9"/>
+      <c r="C11" s="14"/>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
       <c r="J11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+        <v>36</v>
+      </c>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="F10:F11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="I10:I11"/>
     <mergeCell ref="K10:K11"/>
@@ -1066,6 +1064,8 @@
     <mergeCell ref="G9:H9"/>
     <mergeCell ref="C7:K7"/>
     <mergeCell ref="G10:H10"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="F10:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>